<commit_message>
Update Poker Day 10
</commit_message>
<xml_diff>
--- a/Poker_Chip_Tracker.xlsx
+++ b/Poker_Chip_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebas\PycharmProjects\Spade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianrogg/PycharmProjects/Spade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B91641-0E34-432B-AAD0-783B8D9A2227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46945DD2-26A4-1B46-B453-4F03E3E6CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -158,8 +158,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -217,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -586,15 +586,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -624,10 +615,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -635,8 +626,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -659,44 +650,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -705,72 +696,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="132">
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -781,10 +736,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -836,7 +791,7 @@
     <dxf>
       <border>
         <bottom style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -870,6 +825,196 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -879,10 +1024,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -977,10 +1122,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1075,10 +1220,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1173,10 +1318,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1271,10 +1416,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1326,7 +1471,7 @@
     <dxf>
       <border>
         <bottom style="medium">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -1360,163 +1505,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1526,10 +1514,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1624,10 +1612,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1722,10 +1710,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1820,10 +1808,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -1921,10 +1909,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2022,10 +2010,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2123,10 +2111,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2224,10 +2212,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2325,10 +2313,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2421,10 +2409,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color auto="1"/>
@@ -2625,9 +2613,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2651,16 +2639,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$44:$K$44</c:f>
+              <c:f>Overview!$D$44:$L$44</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>18.600000000000001</c:v>
                 </c:pt>
@@ -2684,6 +2675,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>13.400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3500000000000032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2723,9 +2717,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2749,16 +2743,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$45:$K$45</c:f>
+              <c:f>Overview!$D$45:$L$45</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>-16.75</c:v>
                 </c:pt>
@@ -2782,6 +2779,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-15.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-20.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2821,9 +2821,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2847,16 +2847,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$46:$K$46</c:f>
+              <c:f>Overview!$D$46:$L$46</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2880,6 +2883,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-20.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-30.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2919,9 +2925,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2945,16 +2951,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$47:$K$47</c:f>
+              <c:f>Overview!$D$47:$L$47</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -2978,6 +2987,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-21.500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2500000000000036</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3017,9 +3029,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3043,16 +3055,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$48:$K$48</c:f>
+              <c:f>Overview!$D$48:$L$48</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>-17</c:v>
                 </c:pt>
@@ -3076,6 +3091,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.399999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3115,9 +3133,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3141,16 +3159,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$49:$K$49</c:f>
+              <c:f>Overview!$D$49:$L$49</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3173,6 +3194,9 @@
                   <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3215,9 +3239,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3241,16 +3265,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$50:$K$50</c:f>
+              <c:f>Overview!$D$50:$L$50</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>11.15</c:v>
                 </c:pt>
@@ -3274,6 +3301,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>19.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3315,9 +3345,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$K$43</c:f>
+              <c:f>Overview!$D$43:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3341,16 +3371,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$51:$K$51</c:f>
+              <c:f>Overview!$D$51:$L$51</c:f>
               <c:numCache>
-                <c:formatCode>"€"#,##0.00_);[Red]\("€"#,##0.00\)</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3373,6 +3406,9 @@
                   <c:v>10.149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>10.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>10.149999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -3469,7 +3505,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;€&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4232,226 +4268,226 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C371D66B-CC3F-4C51-8D37-5E680D2C583D}" name="Day_11" displayName="Day_11" ref="A1:G9" totalsRowShown="0" headerRowDxfId="40" headerRowBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C371D66B-CC3F-4C51-8D37-5E680D2C583D}" name="Day_11" displayName="Day_11" ref="A1:G9" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{88BD33C2-D366-4E3A-BACB-8AD4974FC7EE}" name="SPIELER" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{795A288E-7844-49A5-9C0F-7B914FE554A1}" name="WIN / LOSS" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{88BD33C2-D366-4E3A-BACB-8AD4974FC7EE}" name="SPIELER" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{795A288E-7844-49A5-9C0F-7B914FE554A1}" name="WIN / LOSS" dataDxfId="68">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{359DC9C0-B875-4031-953F-BCABCF4AB30D}" name="Total Bet" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{359DC9C0-B875-4031-953F-BCABCF4AB30D}" name="Total Bet" dataDxfId="67"/>
     <tableColumn id="4" xr3:uid="{4B50DDA7-FE78-4E07-816E-7412497A7C62}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{C3E17CBB-E15E-4069-84E5-CF0929D090AC}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{FD4799CE-C9DA-4B5D-953E-9936CA67F85E}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{42847FAE-8847-4D3A-996E-3D1E909B239F}" name="100-point chips" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{42847FAE-8847-4D3A-996E-3D1E909B239F}" name="100-point chips" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D4D12BAD-AF3E-41DE-917D-BF45C61A23C6}" name="Day_12" displayName="Day_12" ref="A1:G9" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D4D12BAD-AF3E-41DE-917D-BF45C61A23C6}" name="Day_12" displayName="Day_12" ref="A1:G9" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6175C157-A889-45A6-9A38-D81E65C4D759}" name="SPIELER" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{3AD80E3C-7831-4515-94FB-955B5C9937D8}" name="WIN / LOSS" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{6175C157-A889-45A6-9A38-D81E65C4D759}" name="SPIELER" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{3AD80E3C-7831-4515-94FB-955B5C9937D8}" name="WIN / LOSS" dataDxfId="62">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FC514918-4A2F-473D-90C1-4879AD349286}" name="Total Bet" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{FC514918-4A2F-473D-90C1-4879AD349286}" name="Total Bet" dataDxfId="61"/>
     <tableColumn id="4" xr3:uid="{55149F12-1E8E-4D42-85BE-D2063EE722A9}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{B30FEA25-7090-40A1-8D43-92B224A8D608}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{7D908E53-F7EC-4B91-923E-F1D31A243882}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{ECAA7987-A64D-45B3-917D-416E7B2FE487}" name="100-point chips" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{ECAA7987-A64D-45B3-917D-416E7B2FE487}" name="100-point chips" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{93713727-FEF9-4111-8F6D-27BFE089517D}" name="Day_13" displayName="Day_13" ref="A1:G9" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{93713727-FEF9-4111-8F6D-27BFE089517D}" name="Day_13" displayName="Day_13" ref="A1:G9" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2B9672A9-BE8B-4F6F-98AC-1A48C71E4744}" name="SPIELER" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{D021C65B-5DEE-4F5B-AA43-FE3EC83B4097}" name="WIN / LOSS" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{2B9672A9-BE8B-4F6F-98AC-1A48C71E4744}" name="SPIELER" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{D021C65B-5DEE-4F5B-AA43-FE3EC83B4097}" name="WIN / LOSS" dataDxfId="56">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8241A940-D7ED-4BCF-B186-1DC69BB8F30C}" name="Total Bet" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{8241A940-D7ED-4BCF-B186-1DC69BB8F30C}" name="Total Bet" dataDxfId="55"/>
     <tableColumn id="4" xr3:uid="{6725A0C7-72BA-415D-AC80-2010B3C2ADBE}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{15D91E3F-9D8A-4831-99B3-84BCCF27918A}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{4F451162-D846-4D93-8AB5-A7AC57777D24}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{B77481D9-FC7A-4D1E-99F1-F2584AA16CC8}" name="100-point chips" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{B77481D9-FC7A-4D1E-99F1-F2584AA16CC8}" name="100-point chips" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{522FE926-16F6-49F5-BD76-9F8231AEC269}" name="Day_14" displayName="Day_14" ref="A1:G9" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{522FE926-16F6-49F5-BD76-9F8231AEC269}" name="Day_14" displayName="Day_14" ref="A1:G9" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5CD90ED5-DA9A-43FA-AA9F-D866E2253F5C}" name="SPIELER" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{66AAB64E-CDE3-48EE-AE39-EEBBEFA7EED6}" name="WIN / LOSS" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{5CD90ED5-DA9A-43FA-AA9F-D866E2253F5C}" name="SPIELER" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{66AAB64E-CDE3-48EE-AE39-EEBBEFA7EED6}" name="WIN / LOSS" dataDxfId="50">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A24E5F4A-96AD-420E-A6B0-C891FAC64000}" name="Total Bet" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{A24E5F4A-96AD-420E-A6B0-C891FAC64000}" name="Total Bet" dataDxfId="49"/>
     <tableColumn id="4" xr3:uid="{35588D31-E27A-462D-A091-2A568C381123}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{5702D34C-03D5-4E1A-A46B-3BA6EBE950F0}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{05854272-3983-47A1-825E-530052B87654}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{2717B82E-0190-4449-91A3-16EBFE00AD76}" name="100-point chips" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{2717B82E-0190-4449-91A3-16EBFE00AD76}" name="100-point chips" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{42A3F1B4-4A90-4769-9985-DA06EAFFF23B}" name="Day_15" displayName="Day_15" ref="A1:G9" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{42A3F1B4-4A90-4769-9985-DA06EAFFF23B}" name="Day_15" displayName="Day_15" ref="A1:G9" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00F023A3-EDEA-4FE5-929A-BC20FD1B52D6}" name="SPIELER" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{EA6419C6-FAA7-441A-B3E3-4FC37514B332}" name="WIN / LOSS" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{00F023A3-EDEA-4FE5-929A-BC20FD1B52D6}" name="SPIELER" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{EA6419C6-FAA7-441A-B3E3-4FC37514B332}" name="WIN / LOSS" dataDxfId="44">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{03D4B600-6570-496B-AFF2-823F35D70334}" name="Total Bet" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{03D4B600-6570-496B-AFF2-823F35D70334}" name="Total Bet" dataDxfId="43"/>
     <tableColumn id="4" xr3:uid="{F5ED04A0-E94B-4EDF-B41E-A0998ECB0A2E}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{D3592E76-4B73-4C97-9900-2EBDFA555B3D}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{DD54ADF6-1491-402B-95B7-AB168AEAEF4F}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{5333CD95-239D-4D35-974E-8426AE6349D3}" name="100-point chips" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{5333CD95-239D-4D35-974E-8426AE6349D3}" name="100-point chips" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{7F2A60CB-FD54-2A40-923C-BFD75E7A0945}" name="Table27" displayName="Table27" ref="A1:R9" totalsRowShown="0" headerRowDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{7F2A60CB-FD54-2A40-923C-BFD75E7A0945}" name="Table27" displayName="Table27" ref="A1:R9" totalsRowShown="0" headerRowDxfId="41">
   <autoFilter ref="A1:R9" xr:uid="{7F2A60CB-FD54-2A40-923C-BFD75E7A0945}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R9">
     <sortCondition descending="1" ref="A1:A9"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{92EF8CB9-CB80-E148-A598-263592A13A8C}" name="SPIELER" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{7813C1CF-1A9B-6046-832A-CC2ECA89FAB6}" name="Day 1 " dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{92EF8CB9-CB80-E148-A598-263592A13A8C}" name="SPIELER" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{7813C1CF-1A9B-6046-832A-CC2ECA89FAB6}" name="Day 1 " dataDxfId="39">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B660C4FA-C14B-004F-B492-5035CEBD7DEF}" name="Day 2 " dataDxfId="68">
+    <tableColumn id="3" xr3:uid="{B660C4FA-C14B-004F-B492-5035CEBD7DEF}" name="Day 2 " dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6C4A40C8-4461-204D-B46B-3268E768BF76}" name="Day 3" dataDxfId="67">
+    <tableColumn id="4" xr3:uid="{6C4A40C8-4461-204D-B46B-3268E768BF76}" name="Day 3" dataDxfId="37">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{399A3E3E-1727-0D4F-A7B6-EB361603F2DA}" name="Day 4" dataDxfId="66">
+    <tableColumn id="5" xr3:uid="{399A3E3E-1727-0D4F-A7B6-EB361603F2DA}" name="Day 4" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{72F7BE65-A228-984D-B729-A3258E48126F}" name="Day 5" dataDxfId="65">
+    <tableColumn id="6" xr3:uid="{72F7BE65-A228-984D-B729-A3258E48126F}" name="Day 5" dataDxfId="35">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A0E7C1BE-EC9C-804A-A04D-1BEC5B3371EE}" name="Day 6" dataDxfId="64">
+    <tableColumn id="7" xr3:uid="{A0E7C1BE-EC9C-804A-A04D-1BEC5B3371EE}" name="Day 6" dataDxfId="34">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5AF67BEE-5FB5-B24B-9631-F7CE0DBE78B8}" name="Day 7" dataDxfId="63">
+    <tableColumn id="9" xr3:uid="{5AF67BEE-5FB5-B24B-9631-F7CE0DBE78B8}" name="Day 7" dataDxfId="33">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{89090C79-1C04-B341-BE68-3B5E2E234225}" name="Day 8" dataDxfId="62">
+    <tableColumn id="10" xr3:uid="{89090C79-1C04-B341-BE68-3B5E2E234225}" name="Day 8" dataDxfId="32">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{F382EE00-4228-DE42-840E-5F51A3AB0974}" name="Day 9" dataDxfId="61">
+    <tableColumn id="11" xr3:uid="{F382EE00-4228-DE42-840E-5F51A3AB0974}" name="Day 9" dataDxfId="31">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B0182922-281E-024C-BB09-AD769F3B4FB4}" name="Day 10" dataDxfId="60">
+    <tableColumn id="12" xr3:uid="{B0182922-281E-024C-BB09-AD769F3B4FB4}" name="Day 10" dataDxfId="30">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{99A4EB56-D651-4BC2-A5CA-859F1A3F15B0}" name="Day 11" dataDxfId="10">
+    <tableColumn id="14" xr3:uid="{99A4EB56-D651-4BC2-A5CA-859F1A3F15B0}" name="Day 11" dataDxfId="29">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{F9993AEC-803F-4BA7-968D-107436BB462C}" name="Day 12" dataDxfId="9">
+    <tableColumn id="15" xr3:uid="{F9993AEC-803F-4BA7-968D-107436BB462C}" name="Day 12" dataDxfId="28">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A5F9D543-03D6-4394-A34A-49965C66E32F}" name="Day 13" dataDxfId="8">
+    <tableColumn id="16" xr3:uid="{A5F9D543-03D6-4394-A34A-49965C66E32F}" name="Day 13" dataDxfId="27">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{F80688AC-2797-4B24-810A-7953A26A1886}" name="Day 14" dataDxfId="7">
+    <tableColumn id="17" xr3:uid="{F80688AC-2797-4B24-810A-7953A26A1886}" name="Day 14" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{0C41B488-8226-4607-9626-810AA705FB58}" name="Day 15" dataDxfId="6">
+    <tableColumn id="18" xr3:uid="{0C41B488-8226-4607-9626-810AA705FB58}" name="Day 15" dataDxfId="25">
       <calculatedColumnFormula>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E5EE923F-05E4-6546-B9F0-0B9333029A6A}" name="Σ" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{E5EE923F-05E4-6546-B9F0-0B9333029A6A}" name="Σ" dataDxfId="24">
       <calculatedColumnFormula>SUM(B2:P2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{96EC457F-8EF5-9140-8717-7527BFB349F9}" name="SPIELER2" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{96EC457F-8EF5-9140-8717-7527BFB349F9}" name="SPIELER2" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A90A8FC3-0A04-6543-8040-AB296FF02CAB}" name="Table273" displayName="Table273" ref="A43:Q51" totalsRowShown="0" headerRowDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A90A8FC3-0A04-6543-8040-AB296FF02CAB}" name="Table273" displayName="Table273" ref="A43:Q51" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A43:Q51" xr:uid="{A90A8FC3-0A04-6543-8040-AB296FF02CAB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:Q51">
     <sortCondition descending="1" ref="A43:A51"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{D4A63321-B08A-B943-AC60-4A85C9318E90}" name="SPIELER" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{D4A63321-B08A-B943-AC60-4A85C9318E90}" name="SPIELER" dataDxfId="21"/>
     <tableColumn id="9" xr3:uid="{DE305DD2-BCB7-EC40-AE00-3B7E06363F66}" name="Day 0">
       <calculatedColumnFormula>VLOOKUP(#REF!,Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C4A08EA6-C09B-6C44-818F-6D9C0EBD988D}" name="Day 1 " dataDxfId="56">
+    <tableColumn id="2" xr3:uid="{C4A08EA6-C09B-6C44-818F-6D9C0EBD988D}" name="Day 1 " dataDxfId="20">
       <calculatedColumnFormula>B44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6D0ED243-E740-BE43-8908-60F2BCA06363}" name="Day 2 " dataDxfId="55">
+    <tableColumn id="3" xr3:uid="{6D0ED243-E740-BE43-8908-60F2BCA06363}" name="Day 2 " dataDxfId="19">
       <calculatedColumnFormula>C44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5FF8194E-5DF4-0446-91F0-D45A23CB6151}" name="Day 3" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{5FF8194E-5DF4-0446-91F0-D45A23CB6151}" name="Day 3" dataDxfId="18">
       <calculatedColumnFormula>D44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B37B4B39-B8AF-F845-8DC2-BF41717C6C3E}" name="Day 4" dataDxfId="53">
+    <tableColumn id="5" xr3:uid="{B37B4B39-B8AF-F845-8DC2-BF41717C6C3E}" name="Day 4" dataDxfId="17">
       <calculatedColumnFormula>E44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{93E03325-9DD5-6C43-9F4C-A12288F6E429}" name="Day 5" dataDxfId="52">
+    <tableColumn id="6" xr3:uid="{93E03325-9DD5-6C43-9F4C-A12288F6E429}" name="Day 5" dataDxfId="16">
       <calculatedColumnFormula>F44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{68CD8288-38D9-8D44-9425-B4C1D9B32EBA}" name="Day 6" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{68CD8288-38D9-8D44-9425-B4C1D9B32EBA}" name="Day 6" dataDxfId="15">
       <calculatedColumnFormula>G44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{07BDFF4C-FBC4-4642-8E6F-C52CAD418185}" name="Day 7" dataDxfId="50">
+    <tableColumn id="8" xr3:uid="{07BDFF4C-FBC4-4642-8E6F-C52CAD418185}" name="Day 7" dataDxfId="14">
       <calculatedColumnFormula>H44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{FF38180E-6AFB-CC44-95D8-531B1A543616}" name="Day 8" dataDxfId="49">
+    <tableColumn id="10" xr3:uid="{FF38180E-6AFB-CC44-95D8-531B1A543616}" name="Day 8" dataDxfId="13">
       <calculatedColumnFormula>I44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9CDD3E59-4169-474E-92DD-4FB009A76A55}" name="Day 9" dataDxfId="48">
+    <tableColumn id="11" xr3:uid="{9CDD3E59-4169-474E-92DD-4FB009A76A55}" name="Day 9" dataDxfId="12">
       <calculatedColumnFormula>J44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{8234F178-5432-FE46-A39A-77CBB786AB45}" name="Day 10" dataDxfId="47">
+    <tableColumn id="12" xr3:uid="{8234F178-5432-FE46-A39A-77CBB786AB45}" name="Day 10" dataDxfId="11">
       <calculatedColumnFormula>K44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{31635AC4-8DEA-4929-A2B2-E706550DB5E4}" name="Day 11" dataDxfId="5">
+    <tableColumn id="13" xr3:uid="{31635AC4-8DEA-4929-A2B2-E706550DB5E4}" name="Day 11" dataDxfId="10">
       <calculatedColumnFormula>L44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{CFF24DE5-134D-4DCF-90A8-6C8E98A91C1A}" name="Day 12" dataDxfId="4">
+    <tableColumn id="14" xr3:uid="{CFF24DE5-134D-4DCF-90A8-6C8E98A91C1A}" name="Day 12" dataDxfId="9">
       <calculatedColumnFormula>M44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B600E539-7E07-495C-828D-18541BFB7ACD}" name="Day 13" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{B600E539-7E07-495C-828D-18541BFB7ACD}" name="Day 13" dataDxfId="8">
       <calculatedColumnFormula>N44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{B4159E44-30A3-47C0-9D37-9D4466EE716B}" name="Day 14" dataDxfId="2">
+    <tableColumn id="16" xr3:uid="{B4159E44-30A3-47C0-9D37-9D4466EE716B}" name="Day 14" dataDxfId="7">
       <calculatedColumnFormula>O44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{9FB17180-AF73-4092-9270-A0939633CB07}" name="Day 15" dataDxfId="1">
+    <tableColumn id="17" xr3:uid="{9FB17180-AF73-4092-9270-A0939633CB07}" name="Day 15" dataDxfId="6">
       <calculatedColumnFormula>P44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4460,21 +4496,21 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G9" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="2">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{8B9ED35C-24C5-6844-B237-43D33B16196A}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{E4DF8B73-C3F7-C348-BBAC-F5854E3538E0}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{0FF71DCD-2492-7143-B294-2EFF6F4A222D}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4942,17 +4978,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -4975,7 +5011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -4999,7 +5035,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -5023,7 +5059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -5047,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -5071,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -5095,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -5119,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5143,7 +5179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -5167,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -5176,7 +5212,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -5218,21 +5254,21 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="258" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -5255,88 +5291,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="18">
         <f t="shared" ref="B2:B9" si="0">SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</f>
-        <v>0</v>
+        <v>-6.05</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F2" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.100000000000001</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G3" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.25</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G4" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -5351,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -5375,55 +5411,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.25</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-9.0500000000000007</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -5447,7 +5483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -5456,7 +5492,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -5466,26 +5502,26 @@
       </c>
       <c r="C11" s="24">
         <f>SUM(C2:C9)</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" ref="D11:G11" si="1">SUM(D2:D9)</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="F11" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G11" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -5505,17 +5541,17 @@
   <sheetViews>
     <sheetView zoomScale="131" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -5538,7 +5574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -5562,7 +5598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -5586,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -5610,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -5634,7 +5670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -5658,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -5682,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5706,7 +5742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -5730,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -5739,7 +5775,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -5768,7 +5804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -5790,17 +5826,17 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -5823,7 +5859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -5847,7 +5883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -5871,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -5895,7 +5931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -5919,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -5943,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -5967,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5991,7 +6027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -6015,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -6024,7 +6060,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -6053,7 +6089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -6075,17 +6111,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -6108,7 +6144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -6132,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -6156,7 +6192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -6180,7 +6216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -6204,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -6228,7 +6264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -6252,7 +6288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -6276,7 +6312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -6300,7 +6336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -6309,7 +6345,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -6338,7 +6374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -6360,17 +6396,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -6393,7 +6429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -6417,7 +6453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -6441,7 +6477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -6465,7 +6501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -6489,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -6513,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -6537,7 +6573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -6561,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -6585,7 +6621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -6594,7 +6630,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -6623,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -6645,17 +6681,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -6678,7 +6714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -6702,7 +6738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -6726,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -6750,7 +6786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -6774,7 +6810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -6798,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -6822,7 +6858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -6846,7 +6882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -6870,7 +6906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -6879,7 +6915,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -6908,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -6926,16 +6962,16 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="222" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
@@ -6991,7 +7027,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>7</v>
       </c>
@@ -7033,7 +7069,7 @@
       </c>
       <c r="K2" s="43">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-9.0500000000000007</v>
       </c>
       <c r="L2" s="43">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7056,14 +7092,14 @@
         <v>0</v>
       </c>
       <c r="Q2" s="38">
-        <f>SUM(B2:P2)</f>
-        <v>13.400000000000004</v>
+        <f t="shared" ref="Q2:Q9" si="0">SUM(B2:P2)</f>
+        <v>4.3500000000000032</v>
       </c>
       <c r="R2" s="53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="46" t="s">
         <v>4</v>
       </c>
@@ -7105,7 +7141,7 @@
       </c>
       <c r="K3" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-5.25</v>
       </c>
       <c r="L3" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7128,14 +7164,14 @@
         <v>0</v>
       </c>
       <c r="Q3" s="39">
-        <f>SUM(B3:P3)</f>
-        <v>-15.6</v>
+        <f t="shared" si="0"/>
+        <v>-20.85</v>
       </c>
       <c r="R3" s="54" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
         <v>11</v>
       </c>
@@ -7177,7 +7213,7 @@
       </c>
       <c r="K4" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="L4" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7200,14 +7236,14 @@
         <v>0</v>
       </c>
       <c r="Q4" s="39">
-        <f>SUM(B4:P4)</f>
-        <v>-20.2</v>
+        <f t="shared" si="0"/>
+        <v>-30.2</v>
       </c>
       <c r="R4" s="54" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="46" t="s">
         <v>6</v>
       </c>
@@ -7249,7 +7285,7 @@
       </c>
       <c r="K5" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>19.25</v>
       </c>
       <c r="L5" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7272,14 +7308,14 @@
         <v>0</v>
       </c>
       <c r="Q5" s="39">
-        <f>SUM(B5:P5)</f>
-        <v>-21.500000000000004</v>
+        <f t="shared" si="0"/>
+        <v>-2.2500000000000036</v>
       </c>
       <c r="R5" s="54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="46" t="s">
         <v>8</v>
       </c>
@@ -7321,7 +7357,7 @@
       </c>
       <c r="K6" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>11.100000000000001</v>
       </c>
       <c r="L6" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7344,158 +7380,158 @@
         <v>0</v>
       </c>
       <c r="Q6" s="39">
-        <f>SUM(B6:P6)</f>
-        <v>3.2999999999999972</v>
+        <f t="shared" si="0"/>
+        <v>14.399999999999999</v>
       </c>
       <c r="R6" s="54" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="57">
+      <c r="E7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="57">
+      <c r="I7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="57">
+      <c r="J7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="57">
+      <c r="K7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="57">
+      <c r="L7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="M7" s="57">
+      <c r="M7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="57">
+      <c r="N7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P7" s="57">
+      <c r="P7" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="39">
-        <f>SUM(B7:P7)</f>
+        <f t="shared" si="0"/>
         <v>10.7</v>
       </c>
       <c r="R7" s="54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="63">
+      <c r="B8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2.1500000000000004</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>9</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.25</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-6.9499999999999993</v>
       </c>
-      <c r="F8" s="63">
+      <c r="F8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="63">
+      <c r="G8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>1.0500000000000007</v>
       </c>
-      <c r="H8" s="63">
+      <c r="H8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-20</v>
       </c>
-      <c r="I8" s="63">
+      <c r="I8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>22.15</v>
       </c>
-      <c r="J8" s="63">
+      <c r="J8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2.1000000000000014</v>
       </c>
-      <c r="K8" s="63">
+      <c r="K8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="63">
+        <v>-6.05</v>
+      </c>
+      <c r="L8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="63">
+      <c r="M8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="N8" s="63">
+      <c r="N8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="O8" s="63">
+      <c r="O8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P8" s="63">
+      <c r="P8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="Q8" s="39">
-        <f>SUM(B8:P8)</f>
-        <v>19.75</v>
+        <f t="shared" si="0"/>
+        <v>13.7</v>
       </c>
       <c r="R8" s="54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>27</v>
       </c>
@@ -7560,14 +7596,14 @@
         <v>0</v>
       </c>
       <c r="Q9" s="40">
-        <f>SUM(B9:P9)</f>
+        <f t="shared" si="0"/>
         <v>10.149999999999999</v>
       </c>
       <c r="R9" s="55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="37"/>
       <c r="C10" s="34"/>
@@ -7577,7 +7613,7 @@
       <c r="G10" s="37"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>19</v>
       </c>
@@ -7586,23 +7622,23 @@
         <v>8.8817841970012523E-16</v>
       </c>
       <c r="C11" s="23">
-        <f t="shared" ref="C11:G11" si="0">SUM(C2:C9)</f>
+        <f t="shared" ref="C11:G11" si="1">SUM(C2:C9)</f>
         <v>0</v>
       </c>
       <c r="D11" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E11" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F11" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11" s="35">
@@ -7610,43 +7646,43 @@
         <v>0</v>
       </c>
       <c r="I11" s="35">
-        <f t="shared" ref="I11:Q11" si="1">SUM(I2:I9)</f>
+        <f t="shared" ref="I11:K11" si="2">SUM(I2:I9)</f>
         <v>0</v>
       </c>
       <c r="J11" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.7763568394002505E-15</v>
       </c>
       <c r="K11" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>8.8817841970012523E-16</v>
       </c>
       <c r="L11" s="35">
         <f>SUM(L2:L9)</f>
         <v>0</v>
       </c>
       <c r="M11" s="35">
-        <f t="shared" ref="M11:Q11" si="2">SUM(M2:M9)</f>
+        <f t="shared" ref="M11:Q11" si="3">SUM(M2:M9)</f>
         <v>0</v>
       </c>
       <c r="N11" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O11" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P11" s="35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q11" s="35">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -7656,31 +7692,28 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="J38" s="59"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="56" t="s">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="58"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-    </row>
-    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="60"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="60"/>
+    </row>
+    <row r="43" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
         <v>12</v>
       </c>
@@ -7711,29 +7744,29 @@
       <c r="J43" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="K43" s="60" t="s">
+      <c r="K43" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="L43" s="61" t="s">
+      <c r="L43" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="M43" s="62" t="s">
+      <c r="M43" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="N43" s="62" t="s">
+      <c r="N43" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="O43" s="62" t="s">
+      <c r="O43" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="P43" s="62" t="s">
+      <c r="P43" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="Q43" s="62" t="s">
+      <c r="Q43" s="58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="48" t="s">
         <v>7</v>
       </c>
@@ -7776,32 +7809,32 @@
         <f>J44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>13.400000000000004</v>
       </c>
-      <c r="L44" s="57">
+      <c r="L44" s="1">
         <f>K44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.400000000000004</v>
-      </c>
-      <c r="M44" s="57">
+        <v>4.3500000000000032</v>
+      </c>
+      <c r="M44" s="1">
         <f>L44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.400000000000004</v>
-      </c>
-      <c r="N44" s="57">
+        <v>4.3500000000000032</v>
+      </c>
+      <c r="N44" s="1">
         <f>M44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.400000000000004</v>
-      </c>
-      <c r="O44" s="57">
+        <v>-4.6999999999999975</v>
+      </c>
+      <c r="O44" s="1">
         <f>N44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.400000000000004</v>
-      </c>
-      <c r="P44" s="57">
+        <v>-13.749999999999998</v>
+      </c>
+      <c r="P44" s="1">
         <f>O44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.400000000000004</v>
+        <v>-22.799999999999997</v>
       </c>
       <c r="Q44" s="38">
         <f>P44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.400000000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-31.849999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="46" t="s">
         <v>4</v>
       </c>
@@ -7845,32 +7878,32 @@
         <f>J45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-15.6</v>
       </c>
-      <c r="L45" s="57">
+      <c r="L45" s="1">
         <f>K45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-15.6</v>
-      </c>
-      <c r="M45" s="57">
+        <v>-20.85</v>
+      </c>
+      <c r="M45" s="1">
         <f>L45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-15.6</v>
-      </c>
-      <c r="N45" s="57">
+        <v>-20.85</v>
+      </c>
+      <c r="N45" s="1">
         <f>M45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-15.6</v>
-      </c>
-      <c r="O45" s="57">
+        <v>-26.1</v>
+      </c>
+      <c r="O45" s="1">
         <f>N45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-15.6</v>
-      </c>
-      <c r="P45" s="57">
+        <v>-31.35</v>
+      </c>
+      <c r="P45" s="1">
         <f>O45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-15.6</v>
+        <v>-36.6</v>
       </c>
       <c r="Q45" s="39">
         <f>P45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-15.6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-41.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
         <v>11</v>
       </c>
@@ -7913,32 +7946,32 @@
         <f>J46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-20.2</v>
       </c>
-      <c r="L46" s="57">
+      <c r="L46" s="1">
         <f>K46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.2</v>
-      </c>
-      <c r="M46" s="57">
+        <v>-30.2</v>
+      </c>
+      <c r="M46" s="1">
         <f>L46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.2</v>
-      </c>
-      <c r="N46" s="57">
+        <v>-30.2</v>
+      </c>
+      <c r="N46" s="1">
         <f>M46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.2</v>
-      </c>
-      <c r="O46" s="57">
+        <v>-40.200000000000003</v>
+      </c>
+      <c r="O46" s="1">
         <f>N46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.2</v>
-      </c>
-      <c r="P46" s="57">
+        <v>-50.2</v>
+      </c>
+      <c r="P46" s="1">
         <f>O46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.2</v>
+        <v>-60.2</v>
       </c>
       <c r="Q46" s="39">
         <f>P46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-70.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="46" t="s">
         <v>6</v>
       </c>
@@ -7981,32 +8014,32 @@
         <f>J47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-21.500000000000004</v>
       </c>
-      <c r="L47" s="57">
+      <c r="L47" s="1">
         <f>K47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-21.500000000000004</v>
-      </c>
-      <c r="M47" s="57">
+        <v>-2.2500000000000036</v>
+      </c>
+      <c r="M47" s="1">
         <f>L47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-21.500000000000004</v>
-      </c>
-      <c r="N47" s="57">
+        <v>-2.2500000000000036</v>
+      </c>
+      <c r="N47" s="1">
         <f>M47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-21.500000000000004</v>
-      </c>
-      <c r="O47" s="57">
+        <v>16.999999999999996</v>
+      </c>
+      <c r="O47" s="1">
         <f>N47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-21.500000000000004</v>
-      </c>
-      <c r="P47" s="57">
+        <v>36.25</v>
+      </c>
+      <c r="P47" s="1">
         <f>O47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-21.500000000000004</v>
+        <v>55.5</v>
       </c>
       <c r="Q47" s="39">
         <f>P47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-21.500000000000004</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>74.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
         <v>8</v>
       </c>
@@ -8049,91 +8082,91 @@
         <f>J48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>3.2999999999999972</v>
       </c>
-      <c r="L48" s="57">
+      <c r="L48" s="1">
         <f>K48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>3.2999999999999972</v>
-      </c>
-      <c r="M48" s="57">
+        <v>14.399999999999999</v>
+      </c>
+      <c r="M48" s="1">
         <f>L48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>3.2999999999999972</v>
-      </c>
-      <c r="N48" s="57">
+        <v>14.399999999999999</v>
+      </c>
+      <c r="N48" s="1">
         <f>M48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>3.2999999999999972</v>
-      </c>
-      <c r="O48" s="57">
+        <v>25.5</v>
+      </c>
+      <c r="O48" s="1">
         <f>N48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>3.2999999999999972</v>
-      </c>
-      <c r="P48" s="57">
+        <v>36.6</v>
+      </c>
+      <c r="P48" s="1">
         <f>O48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>3.2999999999999972</v>
+        <v>47.7</v>
       </c>
       <c r="Q48" s="39">
         <f>P48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>3.2999999999999972</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>58.800000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="57">
-        <v>0</v>
-      </c>
-      <c r="C49" s="57">
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
         <f>B49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="D49" s="57">
+      <c r="D49" s="1">
         <f>C49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="E49" s="57">
+      <c r="E49" s="1">
         <f>D49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F49" s="57">
+      <c r="F49" s="1">
         <f>E49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="G49" s="57">
+      <c r="G49" s="1">
         <f>F49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="H49" s="57">
+      <c r="H49" s="1">
         <f>G49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="I49" s="57">
+      <c r="I49" s="1">
         <f>H49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="J49" s="57">
+      <c r="J49" s="1">
         <f>I49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="K49" s="57">
+      <c r="K49" s="1">
         <f>J49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="L49" s="57">
+      <c r="L49" s="1">
         <f>K49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="M49" s="57">
+      <c r="M49" s="1">
         <f>L49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="N49" s="57">
+      <c r="N49" s="1">
         <f>M49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="O49" s="57">
+      <c r="O49" s="1">
         <f>N49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
-      <c r="P49" s="57">
+      <c r="P49" s="1">
         <f>O49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
@@ -8142,75 +8175,75 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="63">
-        <v>0</v>
-      </c>
-      <c r="C50" s="63">
+      <c r="B50" s="21">
+        <v>0</v>
+      </c>
+      <c r="C50" s="21">
         <f>B50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2.1500000000000004</v>
       </c>
-      <c r="D50" s="63">
+      <c r="D50" s="21">
         <f>C50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>11.15</v>
       </c>
-      <c r="E50" s="63">
+      <c r="E50" s="21">
         <f>D50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>21.4</v>
       </c>
-      <c r="F50" s="63">
+      <c r="F50" s="21">
         <f>E50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>14.45</v>
       </c>
-      <c r="G50" s="63">
+      <c r="G50" s="21">
         <f>F50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>14.45</v>
       </c>
-      <c r="H50" s="63">
+      <c r="H50" s="21">
         <f>G50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>15.5</v>
       </c>
-      <c r="I50" s="57">
+      <c r="I50" s="1">
         <f>H50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-4.5</v>
       </c>
-      <c r="J50" s="57">
+      <c r="J50" s="1">
         <f>I50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>17.649999999999999</v>
       </c>
-      <c r="K50" s="57">
+      <c r="K50" s="1">
         <f>J50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>19.75</v>
       </c>
-      <c r="L50" s="57">
+      <c r="L50" s="1">
         <f>K50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>19.75</v>
-      </c>
-      <c r="M50" s="57">
+        <v>13.7</v>
+      </c>
+      <c r="M50" s="1">
         <f>L50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>19.75</v>
-      </c>
-      <c r="N50" s="57">
+        <v>13.7</v>
+      </c>
+      <c r="N50" s="1">
         <f>M50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>19.75</v>
-      </c>
-      <c r="O50" s="57">
+        <v>7.6499999999999995</v>
+      </c>
+      <c r="O50" s="1">
         <f>N50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>19.75</v>
-      </c>
-      <c r="P50" s="57">
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="P50" s="1">
         <f>O50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>19.75</v>
+        <v>-4.45</v>
       </c>
       <c r="Q50" s="39">
         <f>P50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-10.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
         <v>27</v>
       </c>
@@ -8284,6 +8317,9 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B44:B51" calculatedColumn="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -8301,17 +8337,17 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -8334,7 +8370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -8358,7 +8394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -8382,7 +8418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -8406,7 +8442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -8430,7 +8466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -8454,7 +8490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -8478,7 +8514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -8502,7 +8538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -8526,7 +8562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -8535,7 +8571,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -8564,7 +8600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -8586,17 +8622,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -8619,7 +8655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -8643,7 +8679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -8667,7 +8703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -8691,7 +8727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -8715,7 +8751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -8739,7 +8775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -8763,7 +8799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -8787,7 +8823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -8811,7 +8847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -8820,7 +8856,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -8866,17 +8902,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -8899,7 +8935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -8923,7 +8959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -8947,7 +8983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -8971,7 +9007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -8995,7 +9031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -9019,7 +9055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -9043,7 +9079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -9067,7 +9103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -9091,7 +9127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -9100,7 +9136,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -9146,17 +9182,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -9179,7 +9215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -9203,7 +9239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -9227,7 +9263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -9251,7 +9287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -9275,7 +9311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -9299,7 +9335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -9323,7 +9359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -9347,7 +9383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -9371,7 +9407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -9380,7 +9416,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -9426,17 +9462,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -9459,7 +9495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
@@ -9483,7 +9519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -9507,7 +9543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -9531,7 +9567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -9555,7 +9591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -9579,7 +9615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -9603,7 +9639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -9627,7 +9663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
@@ -9651,7 +9687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -9660,7 +9696,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -9706,17 +9742,17 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -9739,7 +9775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -9763,7 +9799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -9787,7 +9823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -9811,7 +9847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -9835,7 +9871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -9859,7 +9895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -9883,7 +9919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -9907,7 +9943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -9931,7 +9967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -9940,7 +9976,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>19</v>
       </c>
@@ -9986,17 +10022,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -10019,7 +10055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -10043,7 +10079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -10067,7 +10103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -10091,7 +10127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -10115,7 +10151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -10139,7 +10175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -10163,7 +10199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -10187,7 +10223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -10211,7 +10247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -10220,7 +10256,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -10249,7 +10285,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -10271,17 +10307,17 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -10304,7 +10340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -10328,7 +10364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -10352,7 +10388,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -10376,7 +10412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -10400,7 +10436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -10424,7 +10460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -10448,7 +10484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -10472,7 +10508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -10496,7 +10532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -10505,7 +10541,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -10534,7 +10570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>
@@ -10556,17 +10592,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -10589,7 +10625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
@@ -10613,7 +10649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -10637,7 +10673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -10661,7 +10697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -10685,7 +10721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -10709,7 +10745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -10733,7 +10769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -10757,7 +10793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -10781,7 +10817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="30"/>
       <c r="C10" s="27"/>
@@ -10790,7 +10826,7 @@
       <c r="F10" s="32"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>19</v>
       </c>
@@ -10819,7 +10855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="2"/>
       <c r="F12" s="10"/>

</xml_diff>

<commit_message>
Add dynamic Excel data syncing for lineChartDataDashboard
Introduced functionality to update `lineChartDataDashboard` directly from an Excel sheet using the `xlsx` library. This includes creating a script to process data and a new dependency in `package.json`. Additionally, updated chart categories to support 11 days of data.
</commit_message>
<xml_diff>
--- a/Poker_Chip_Tracker.xlsx
+++ b/Poker_Chip_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianrogg/PycharmProjects/Spade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46945DD2-26A4-1B46-B453-4F03E3E6CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C82C00E-2163-C843-AB99-9A706A1784B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="42">
   <si>
     <t>5-point chips</t>
   </si>
@@ -151,6 +151,30 @@
   </si>
   <si>
     <t>Day 15</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Matthi</t>
+  </si>
+  <si>
+    <t>Markus</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Jura Jonas</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Eliah</t>
   </si>
 </sst>
 </file>
@@ -615,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -721,11 +745,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="132">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -823,18 +862,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
@@ -2594,7 +2621,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SEBASTIAN</c:v>
+                  <c:v>Sebastian</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2698,7 +2725,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PAUL</c:v>
+                  <c:v>Paul</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2802,7 +2829,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MATTHI</c:v>
+                  <c:v>Matthi</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2906,7 +2933,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MARKUS</c:v>
+                  <c:v>Markus</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3010,7 +3037,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LUCA</c:v>
+                  <c:v>Luca</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3114,7 +3141,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>JURA JONAS</c:v>
+                  <c:v>Jura Jonas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3218,7 +3245,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>JONAS</c:v>
+                  <c:v>Jonas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3324,7 +3351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ELIAH</c:v>
+                  <c:v>Eliah</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4435,7 +4462,7 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A90A8FC3-0A04-6543-8040-AB296FF02CAB}" name="Table273" displayName="Table273" ref="A43:Q51" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A90A8FC3-0A04-6543-8040-AB296FF02CAB}" name="MovingSum" displayName="MovingSum" ref="A43:Q51" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A43:Q51" xr:uid="{A90A8FC3-0A04-6543-8040-AB296FF02CAB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:Q51">
     <sortCondition descending="1" ref="A43:A51"/>
@@ -4446,49 +4473,49 @@
       <calculatedColumnFormula>VLOOKUP(#REF!,Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{C4A08EA6-C09B-6C44-818F-6D9C0EBD988D}" name="Day 1 " dataDxfId="20">
-      <calculatedColumnFormula>B44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>B44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{6D0ED243-E740-BE43-8908-60F2BCA06363}" name="Day 2 " dataDxfId="19">
-      <calculatedColumnFormula>C44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>C44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{5FF8194E-5DF4-0446-91F0-D45A23CB6151}" name="Day 3" dataDxfId="18">
-      <calculatedColumnFormula>D44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>D44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{B37B4B39-B8AF-F845-8DC2-BF41717C6C3E}" name="Day 4" dataDxfId="17">
-      <calculatedColumnFormula>E44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>E44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{93E03325-9DD5-6C43-9F4C-A12288F6E429}" name="Day 5" dataDxfId="16">
-      <calculatedColumnFormula>F44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>F44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{68CD8288-38D9-8D44-9425-B4C1D9B32EBA}" name="Day 6" dataDxfId="15">
-      <calculatedColumnFormula>G44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>G44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{07BDFF4C-FBC4-4642-8E6F-C52CAD418185}" name="Day 7" dataDxfId="14">
-      <calculatedColumnFormula>H44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>H44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{FF38180E-6AFB-CC44-95D8-531B1A543616}" name="Day 8" dataDxfId="13">
-      <calculatedColumnFormula>I44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>I44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{9CDD3E59-4169-474E-92DD-4FB009A76A55}" name="Day 9" dataDxfId="12">
-      <calculatedColumnFormula>J44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>J44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{8234F178-5432-FE46-A39A-77CBB786AB45}" name="Day 10" dataDxfId="11">
-      <calculatedColumnFormula>K44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>K44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{31635AC4-8DEA-4929-A2B2-E706550DB5E4}" name="Day 11" dataDxfId="10">
-      <calculatedColumnFormula>L44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+      <calculatedColumnFormula>L44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{CFF24DE5-134D-4DCF-90A8-6C8E98A91C1A}" name="Day 12" dataDxfId="9">
-      <calculatedColumnFormula>M44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="14" xr3:uid="{CFF24DE5-134D-4DCF-90A8-6C8E98A91C1A}" name="Day 12" dataDxfId="3">
+      <calculatedColumnFormula>M44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B600E539-7E07-495C-828D-18541BFB7ACD}" name="Day 13" dataDxfId="8">
-      <calculatedColumnFormula>N44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="15" xr3:uid="{B600E539-7E07-495C-828D-18541BFB7ACD}" name="Day 13" dataDxfId="2">
+      <calculatedColumnFormula>N44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{B4159E44-30A3-47C0-9D37-9D4466EE716B}" name="Day 14" dataDxfId="7">
-      <calculatedColumnFormula>O44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{B4159E44-30A3-47C0-9D37-9D4466EE716B}" name="Day 14" dataDxfId="1">
+      <calculatedColumnFormula>O44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{9FB17180-AF73-4092-9270-A0939633CB07}" name="Day 15" dataDxfId="6">
-      <calculatedColumnFormula>P44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{9FB17180-AF73-4092-9270-A0939633CB07}" name="Day 15" dataDxfId="0">
+      <calculatedColumnFormula>P44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4496,21 +4523,21 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G9" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="6">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{8B9ED35C-24C5-6844-B237-43D33B16196A}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{E4DF8B73-C3F7-C348-BBAC-F5854E3538E0}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{0FF71DCD-2492-7143-B294-2EFF6F4A222D}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4975,7 +5002,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5254,8 +5281,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="258" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="212" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6962,8 +6989,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="222" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7691,6 +7718,12 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B37" s="62"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C39" s="62"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="59" t="s">
@@ -7768,546 +7801,546 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="48" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B44" s="43">
         <v>0</v>
       </c>
       <c r="C44" s="43">
-        <f>B44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>11.3</v>
       </c>
       <c r="D44" s="43">
-        <f>C44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>18.600000000000001</v>
       </c>
       <c r="E44" s="43">
-        <f>D44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>8.0000000000000018</v>
       </c>
       <c r="F44" s="43">
-        <f>E44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-0.64999999999999858</v>
       </c>
       <c r="G44" s="43">
-        <f>F44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>4.1500000000000021</v>
       </c>
       <c r="H44" s="43">
-        <f>G44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>8.6500000000000021</v>
       </c>
       <c r="I44" s="43">
-        <f>H44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>28.200000000000003</v>
       </c>
       <c r="J44" s="43">
-        <f>I44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>11.000000000000004</v>
       </c>
       <c r="K44" s="1">
-        <f>J44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>13.400000000000004</v>
       </c>
-      <c r="L44" s="1">
-        <f>K44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+      <c r="L44" s="63">
+        <f>K44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>4.3500000000000032</v>
       </c>
       <c r="M44" s="1">
-        <f>L44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>4.3500000000000032</v>
       </c>
       <c r="N44" s="1">
-        <f>M44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-4.6999999999999975</v>
+        <f>M44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>4.3500000000000032</v>
       </c>
       <c r="O44" s="1">
-        <f>N44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-13.749999999999998</v>
+        <f>N44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>4.3500000000000032</v>
       </c>
       <c r="P44" s="1">
-        <f>O44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-22.799999999999997</v>
+        <f>O44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>4.3500000000000032</v>
       </c>
       <c r="Q44" s="38">
-        <f>P44+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-31.849999999999998</v>
+        <f>P44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>4.3500000000000032</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="46" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B45" s="1">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="C45" s="1">
-        <f>B45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-10</v>
       </c>
       <c r="D45" s="1">
-        <f>C45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-16.75</v>
       </c>
       <c r="E45" s="1">
-        <f>D45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F45" s="1">
-        <f>E45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-1.0499999999999998</v>
       </c>
       <c r="G45" s="1">
-        <f>F45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-11.05</v>
       </c>
       <c r="H45" s="1">
-        <f>G45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-21.75</v>
       </c>
       <c r="I45" s="1">
-        <f>H45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-9.8999999999999986</v>
       </c>
       <c r="J45" s="1">
-        <f>I45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-9.5499999999999989</v>
       </c>
       <c r="K45" s="1">
-        <f>J45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-15.6</v>
       </c>
       <c r="L45" s="1">
-        <f>K45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-20.85</v>
       </c>
       <c r="M45" s="1">
-        <f>L45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-20.85</v>
       </c>
       <c r="N45" s="1">
-        <f>M45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-26.1</v>
+        <f>M45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-20.85</v>
       </c>
       <c r="O45" s="1">
-        <f>N45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-31.35</v>
+        <f>N45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-20.85</v>
       </c>
       <c r="P45" s="1">
-        <f>O45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-36.6</v>
+        <f>O45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-20.85</v>
       </c>
       <c r="Q45" s="39">
-        <f>P45+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-41.85</v>
+        <f>P45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-20.85</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B46" s="21">
         <v>0</v>
       </c>
       <c r="C46" s="21">
-        <f>B46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D46" s="21">
-        <f>C46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="E46" s="21">
-        <f>D46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-10</v>
       </c>
       <c r="F46" s="21">
-        <f>E46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-14</v>
       </c>
       <c r="G46" s="21">
-        <f>F46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-14</v>
       </c>
       <c r="H46" s="21">
-        <f>G46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-10.199999999999999</v>
       </c>
       <c r="I46" s="1">
-        <f>H46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-10.199999999999999</v>
       </c>
       <c r="J46" s="1">
-        <f>I46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-22.15</v>
       </c>
-      <c r="K46" s="1">
-        <f>J46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+      <c r="K46" s="61">
+        <f>J46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-20.2</v>
       </c>
       <c r="L46" s="1">
-        <f>K46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-30.2</v>
       </c>
       <c r="M46" s="1">
-        <f>L46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-30.2</v>
       </c>
       <c r="N46" s="1">
-        <f>M46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-40.200000000000003</v>
+        <f>M46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-30.2</v>
       </c>
       <c r="O46" s="1">
-        <f>N46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-50.2</v>
+        <f>N46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-30.2</v>
       </c>
       <c r="P46" s="1">
-        <f>O46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-60.2</v>
+        <f>O46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-30.2</v>
       </c>
       <c r="Q46" s="39">
-        <f>P46+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-70.2</v>
+        <f>P46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-30.2</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="46" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B47" s="21">
         <v>0</v>
       </c>
       <c r="C47" s="21">
-        <f>B47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D47" s="21">
-        <f>C47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E47" s="21">
-        <f>D47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-5.5</v>
       </c>
       <c r="F47" s="21">
-        <f>E47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-5.5</v>
       </c>
       <c r="G47" s="21">
-        <f>F47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2.1999999999999993</v>
       </c>
       <c r="H47" s="21">
-        <f>G47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2.1999999999999993</v>
       </c>
       <c r="I47" s="1">
-        <f>H47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-7.9500000000000011</v>
       </c>
       <c r="J47" s="1">
-        <f>I47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-37.950000000000003</v>
       </c>
       <c r="K47" s="1">
-        <f>J47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-21.500000000000004</v>
       </c>
       <c r="L47" s="1">
-        <f>K47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-2.2500000000000036</v>
       </c>
       <c r="M47" s="1">
-        <f>L47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-2.2500000000000036</v>
       </c>
       <c r="N47" s="1">
-        <f>M47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>16.999999999999996</v>
+        <f>M47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-2.2500000000000036</v>
       </c>
       <c r="O47" s="1">
-        <f>N47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>36.25</v>
+        <f>N47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-2.2500000000000036</v>
       </c>
       <c r="P47" s="1">
-        <f>O47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>55.5</v>
+        <f>O47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-2.2500000000000036</v>
       </c>
       <c r="Q47" s="39">
-        <f>P47+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>74.75</v>
+        <f>P47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>-2.2500000000000036</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="46" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B48" s="21">
         <v>0</v>
       </c>
       <c r="C48" s="21">
-        <f>B48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-3.45</v>
       </c>
       <c r="D48" s="21">
-        <f>C48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-17</v>
       </c>
       <c r="E48" s="21">
-        <f>D48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-15.9</v>
       </c>
       <c r="F48" s="21">
-        <f>E48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-3.9500000000000011</v>
       </c>
       <c r="G48" s="21">
-        <f>F48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-6.4500000000000011</v>
       </c>
       <c r="H48" s="21">
-        <f>G48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-15.250000000000002</v>
       </c>
       <c r="I48" s="1">
-        <f>H48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-16.5</v>
       </c>
       <c r="J48" s="1">
-        <f>I48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>20.149999999999999</v>
       </c>
       <c r="K48" s="1">
-        <f>J48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>3.2999999999999972</v>
       </c>
       <c r="L48" s="1">
-        <f>K48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>14.399999999999999</v>
       </c>
       <c r="M48" s="1">
-        <f>L48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>14.399999999999999</v>
       </c>
       <c r="N48" s="1">
-        <f>M48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>25.5</v>
+        <f>M48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>14.399999999999999</v>
       </c>
       <c r="O48" s="1">
-        <f>N48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>36.6</v>
+        <f>N48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>14.399999999999999</v>
       </c>
       <c r="P48" s="1">
-        <f>O48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>47.7</v>
+        <f>O48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>14.399999999999999</v>
       </c>
       <c r="Q48" s="39">
-        <f>P48+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>58.800000000000004</v>
+        <f>P48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>14.399999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="46" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
       </c>
       <c r="C49" s="1">
-        <f>B49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D49" s="1">
-        <f>C49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="E49" s="1">
-        <f>D49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="F49" s="1">
-        <f>E49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="G49" s="1">
-        <f>F49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="H49" s="1">
-        <f>G49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="I49" s="1">
-        <f>H49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="J49" s="1">
-        <f>I49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="K49" s="1">
-        <f>J49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="L49" s="1">
-        <f>K49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="M49" s="1">
-        <f>L49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="N49" s="1">
-        <f>M49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>M49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="O49" s="1">
-        <f>N49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>N49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="P49" s="1">
-        <f>O49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>O49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
       <c r="Q49" s="39">
-        <f>P49+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>P49+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.7</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="46" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B50" s="21">
         <v>0</v>
       </c>
       <c r="C50" s="21">
-        <f>B50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>2.1500000000000004</v>
       </c>
       <c r="D50" s="21">
-        <f>C50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>11.15</v>
       </c>
       <c r="E50" s="21">
-        <f>D50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>21.4</v>
       </c>
       <c r="F50" s="21">
-        <f>E50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>14.45</v>
       </c>
       <c r="G50" s="21">
-        <f>F50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>14.45</v>
       </c>
       <c r="H50" s="21">
-        <f>G50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>15.5</v>
       </c>
       <c r="I50" s="1">
-        <f>H50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-4.5</v>
       </c>
       <c r="J50" s="1">
-        <f>I50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>17.649999999999999</v>
       </c>
       <c r="K50" s="1">
-        <f>J50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>19.75</v>
       </c>
       <c r="L50" s="1">
-        <f>K50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>13.7</v>
       </c>
       <c r="M50" s="1">
-        <f>L50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>13.7</v>
       </c>
       <c r="N50" s="1">
-        <f>M50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>7.6499999999999995</v>
+        <f>M50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>13.7</v>
       </c>
       <c r="O50" s="1">
-        <f>N50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>1.5999999999999996</v>
+        <f>N50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>13.7</v>
       </c>
       <c r="P50" s="1">
-        <f>O50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-4.45</v>
+        <f>O50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>13.7</v>
       </c>
       <c r="Q50" s="39">
-        <f>P50+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-10.5</v>
+        <f>P50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <v>13.7</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B51" s="50">
         <v>0</v>
       </c>
       <c r="C51" s="50">
-        <f>B51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>B51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_1[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="D51" s="50">
-        <f>C51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>C51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_2[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="E51" s="50">
-        <f>D51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>D51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_3[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="F51" s="50">
-        <f>E51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>E51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_4[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G51" s="50">
-        <f>F51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>F51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_5[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="H51" s="50">
-        <f>G51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>G51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_6[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="I51" s="6">
-        <f>H51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>H51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_7[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="J51" s="6">
-        <f>I51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>I51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="K51" s="6">
-        <f>J51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>J51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="L51" s="6">
-        <f>K51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>K51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="M51" s="6">
-        <f>L51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>L51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="N51" s="6">
-        <f>M51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>M51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="O51" s="6">
-        <f>N51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>N51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="P51" s="6">
-        <f>O51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>O51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
       <c r="Q51" s="40">
-        <f>P51+VLOOKUP(Table273[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
+        <f>P51+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>10.149999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add svg spade logo and fix fullscreen buttons, skibidi scroll, Day 13 Poker_Chip_Tracker.xlsx
</commit_message>
<xml_diff>
--- a/Poker_Chip_Tracker.xlsx
+++ b/Poker_Chip_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianrogg/PycharmProjects/Spade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C82C00E-2163-C843-AB99-9A706A1784B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED9C8B0-4D07-3E45-AF46-F01BBCD4DD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -745,26 +745,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="132">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -862,6 +847,18 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
@@ -2640,9 +2637,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2669,16 +2666,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$44:$L$44</c:f>
+              <c:f>Overview!$D$44:$N$44</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>18.600000000000001</c:v>
                 </c:pt>
@@ -2705,6 +2708,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4.3500000000000032</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2744,9 +2753,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2773,16 +2782,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$45:$L$45</c:f>
+              <c:f>Overview!$D$45:$N$45</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-16.75</c:v>
                 </c:pt>
@@ -2809,6 +2824,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-20.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-40.85</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-70.849999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2848,9 +2869,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2877,16 +2898,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$46:$L$46</c:f>
+              <c:f>Overview!$D$46:$N$46</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2913,6 +2940,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-30.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-34.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-39.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2952,9 +2985,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -2981,16 +3014,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$47:$L$47</c:f>
+              <c:f>Overview!$D$47:$N$47</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -3017,6 +3056,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-2.2500000000000036</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-42.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-39.700000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3056,9 +3101,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3085,16 +3130,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$48:$L$48</c:f>
+              <c:f>Overview!$D$48:$N$48</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-17</c:v>
                 </c:pt>
@@ -3121,6 +3172,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>14.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.349999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3160,9 +3217,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3189,16 +3246,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$49:$L$49</c:f>
+              <c:f>Overview!$D$49:$N$49</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3224,6 +3287,12 @@
                   <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -3266,9 +3335,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3295,16 +3364,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$50:$L$50</c:f>
+              <c:f>Overview!$D$50:$N$50</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>11.15</c:v>
                 </c:pt>
@@ -3331,6 +3406,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3372,9 +3453,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Overview!$D$43:$L$43</c:f>
+              <c:f>Overview!$D$43:$N$43</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>Day 2 </c:v>
                 </c:pt>
@@ -3401,16 +3482,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 12</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overview!$D$51:$L$51</c:f>
+              <c:f>Overview!$D$51:$N$51</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€";[Red]\-#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3436,6 +3523,12 @@
                   <c:v>10.149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>10.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10.149999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -4505,16 +4598,16 @@
     <tableColumn id="13" xr3:uid="{31635AC4-8DEA-4929-A2B2-E706550DB5E4}" name="Day 11" dataDxfId="10">
       <calculatedColumnFormula>L44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{CFF24DE5-134D-4DCF-90A8-6C8E98A91C1A}" name="Day 12" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{CFF24DE5-134D-4DCF-90A8-6C8E98A91C1A}" name="Day 12" dataDxfId="9">
       <calculatedColumnFormula>M44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B600E539-7E07-495C-828D-18541BFB7ACD}" name="Day 13" dataDxfId="2">
+    <tableColumn id="15" xr3:uid="{B600E539-7E07-495C-828D-18541BFB7ACD}" name="Day 13" dataDxfId="8">
       <calculatedColumnFormula>N44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{B4159E44-30A3-47C0-9D37-9D4466EE716B}" name="Day 14" dataDxfId="1">
+    <tableColumn id="16" xr3:uid="{B4159E44-30A3-47C0-9D37-9D4466EE716B}" name="Day 14" dataDxfId="7">
       <calculatedColumnFormula>O44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{9FB17180-AF73-4092-9270-A0939633CB07}" name="Day 15" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{9FB17180-AF73-4092-9270-A0939633CB07}" name="Day 15" dataDxfId="6">
       <calculatedColumnFormula>P44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4523,21 +4616,21 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G9" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}" name="Day_X" displayName="Day_X" ref="A1:G9" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <autoFilter ref="A1:G9" xr:uid="{11542CAC-C0C8-8145-B93D-526D752F01F7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{CAF30B83-9101-DA49-B8E3-FF4E4D4F12E6}" name="SPIELER" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{831EDA8E-0521-854F-89C3-E9F66179C1ED}" name="WIN / LOSS" dataDxfId="2">
       <calculatedColumnFormula>SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{627E6F5A-0CAD-B24D-BFC0-3F65FBBD5A54}" name="Total Bet" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{8B9ED35C-24C5-6844-B237-43D33B16196A}" name="5-point chips"/>
     <tableColumn id="5" xr3:uid="{E4DF8B73-C3F7-C348-BBAC-F5854E3538E0}" name="10-point chips"/>
     <tableColumn id="6" xr3:uid="{0FF71DCD-2492-7143-B294-2EFF6F4A222D}" name="25-point chips"/>
-    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5ECE13F4-1183-1844-B734-A3542720D868}" name="100-point chips" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5566,291 +5659,8 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="18">
-        <f t="shared" ref="B2:B9" si="0">SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="23">
-        <f>SUM(B2:B9)</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="24">
-        <f>SUM(C2:C9)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="25">
-        <f t="shared" ref="D11:G11" si="1">SUM(D2:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="44">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="43"/>
-      <c r="C12" s="2"/>
-      <c r="F12" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585E175D-B90F-46E2-B2DB-535B9433123E}">
-  <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:G12"/>
-  <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScale="263" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5892,22 +5702,22 @@
       </c>
       <c r="B2" s="18">
         <f t="shared" ref="B2:B9" si="0">SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</f>
-        <v>0</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="F2" s="10">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G2" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -5916,22 +5726,22 @@
       </c>
       <c r="B3" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="G3" s="11">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -5940,10 +5750,10 @@
       </c>
       <c r="B4" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -5964,22 +5774,22 @@
       </c>
       <c r="B5" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G5" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -6012,10 +5822,10 @@
       </c>
       <c r="B7" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6036,22 +5846,22 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45.25</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G8" s="11">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -6097,23 +5907,308 @@
       </c>
       <c r="C11" s="24">
         <f>SUM(C2:C9)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" ref="D11:G11" si="1">SUM(D2:D9)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="F11" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G11" s="44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="43"/>
+      <c r="C12" s="2"/>
+      <c r="F12" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585E175D-B90F-46E2-B2DB-535B9433123E}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView zoomScale="215" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="18">
+        <f t="shared" ref="B2:B9" si="0">SUM(D2*0.05,E2*0.1,F2*0.25,G2*1)-C2</f>
+        <v>-1.5999999999999996</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="18">
+        <f t="shared" si="0"/>
+        <v>42.9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>70</v>
+      </c>
+      <c r="F3">
+        <v>68</v>
+      </c>
+      <c r="G3" s="11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="18">
+        <f t="shared" si="0"/>
+        <v>2.5500000000000007</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="18">
+        <f t="shared" si="0"/>
+        <v>-5.3000000000000007</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>14</v>
+      </c>
+      <c r="G5" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="18">
+        <f t="shared" si="0"/>
+        <v>-30</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18">
+        <f t="shared" si="0"/>
+        <v>-8.5500000000000007</v>
+      </c>
+      <c r="C8" s="2">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
+      <c r="G8" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="45"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="23">
+        <f>SUM(B2:B9)</f>
+        <v>-3.5527136788005009E-15</v>
+      </c>
+      <c r="C11" s="24">
+        <f>SUM(C2:C9)</f>
+        <v>110</v>
+      </c>
+      <c r="D11" s="25">
+        <f t="shared" ref="D11:G11" si="1">SUM(D2:D9)</f>
+        <v>66</v>
+      </c>
+      <c r="E11" s="25">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="G11" s="44">
+        <f t="shared" si="1"/>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -6989,8 +7084,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7100,11 +7195,11 @@
       </c>
       <c r="L2" s="43">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>45.25</v>
       </c>
       <c r="M2" s="43">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-8.5500000000000007</v>
       </c>
       <c r="N2" s="43">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7120,7 +7215,7 @@
       </c>
       <c r="Q2" s="38">
         <f t="shared" ref="Q2:Q9" si="0">SUM(B2:P2)</f>
-        <v>4.3500000000000032</v>
+        <v>41.05</v>
       </c>
       <c r="R2" s="53" t="s">
         <v>7</v>
@@ -7172,11 +7267,11 @@
       </c>
       <c r="L3" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="M3" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="N3" s="1">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7192,7 +7287,7 @@
       </c>
       <c r="Q3" s="39">
         <f t="shared" si="0"/>
-        <v>-20.85</v>
+        <v>-70.849999999999994</v>
       </c>
       <c r="R3" s="54" t="s">
         <v>4</v>
@@ -7244,11 +7339,11 @@
       </c>
       <c r="L4" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="M4" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-5.3000000000000007</v>
       </c>
       <c r="N4" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7264,7 +7359,7 @@
       </c>
       <c r="Q4" s="39">
         <f t="shared" si="0"/>
-        <v>-30.2</v>
+        <v>-39.599999999999994</v>
       </c>
       <c r="R4" s="54" t="s">
         <v>11</v>
@@ -7316,11 +7411,11 @@
       </c>
       <c r="L5" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-40</v>
       </c>
       <c r="M5" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>2.5500000000000007</v>
       </c>
       <c r="N5" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7336,7 +7431,7 @@
       </c>
       <c r="Q5" s="39">
         <f t="shared" si="0"/>
-        <v>-2.2500000000000036</v>
+        <v>-39.700000000000003</v>
       </c>
       <c r="R5" s="54" t="s">
         <v>6</v>
@@ -7388,11 +7483,11 @@
       </c>
       <c r="L6" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="M6" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>42.9</v>
       </c>
       <c r="N6" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7408,7 +7503,7 @@
       </c>
       <c r="Q6" s="39">
         <f t="shared" si="0"/>
-        <v>14.399999999999999</v>
+        <v>66.349999999999994</v>
       </c>
       <c r="R6" s="54" t="s">
         <v>8</v>
@@ -7532,11 +7627,11 @@
       </c>
       <c r="L8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="M8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>0</v>
+        <v>-1.5999999999999996</v>
       </c>
       <c r="N8" s="21">
         <f>VLOOKUP(Table27[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
@@ -7552,7 +7647,7 @@
       </c>
       <c r="Q8" s="39">
         <f t="shared" si="0"/>
-        <v>13.7</v>
+        <v>21.9</v>
       </c>
       <c r="R8" s="54" t="s">
         <v>5</v>
@@ -7690,7 +7785,7 @@
       </c>
       <c r="M11" s="35">
         <f t="shared" ref="M11:Q11" si="3">SUM(M2:M9)</f>
-        <v>0</v>
+        <v>1.7763568394002505E-15</v>
       </c>
       <c r="N11" s="35">
         <f t="shared" si="3"/>
@@ -7718,12 +7813,6 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B37" s="62"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C39" s="62"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="59" t="s">
@@ -7842,29 +7931,29 @@
         <f>J44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>13.400000000000004</v>
       </c>
-      <c r="L44" s="63">
+      <c r="L44" s="1">
         <f>K44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_10[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>4.3500000000000032</v>
       </c>
       <c r="M44" s="1">
         <f>L44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>4.3500000000000032</v>
+        <v>49.6</v>
       </c>
       <c r="N44" s="1">
         <f>M44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>4.3500000000000032</v>
+        <v>41.05</v>
       </c>
       <c r="O44" s="1">
         <f>N44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>4.3500000000000032</v>
+        <v>41.05</v>
       </c>
       <c r="P44" s="1">
         <f>O44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>4.3500000000000032</v>
+        <v>41.05</v>
       </c>
       <c r="Q44" s="38">
         <f>P44+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>4.3500000000000032</v>
+        <v>41.05</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
@@ -7917,23 +8006,23 @@
       </c>
       <c r="M45" s="1">
         <f>L45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.85</v>
+        <v>-40.85</v>
       </c>
       <c r="N45" s="1">
         <f>M45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.85</v>
+        <v>-70.849999999999994</v>
       </c>
       <c r="O45" s="1">
         <f>N45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.85</v>
+        <v>-70.849999999999994</v>
       </c>
       <c r="P45" s="1">
         <f>O45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.85</v>
+        <v>-70.849999999999994</v>
       </c>
       <c r="Q45" s="39">
         <f>P45+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-20.85</v>
+        <v>-70.849999999999994</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -7975,7 +8064,7 @@
         <f>I46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_8[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-22.15</v>
       </c>
-      <c r="K46" s="61">
+      <c r="K46" s="1">
         <f>J46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_9[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
         <v>-20.2</v>
       </c>
@@ -7985,23 +8074,23 @@
       </c>
       <c r="M46" s="1">
         <f>L46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-30.2</v>
+        <v>-34.299999999999997</v>
       </c>
       <c r="N46" s="1">
         <f>M46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-30.2</v>
+        <v>-39.599999999999994</v>
       </c>
       <c r="O46" s="1">
         <f>N46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-30.2</v>
+        <v>-39.599999999999994</v>
       </c>
       <c r="P46" s="1">
         <f>O46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-30.2</v>
+        <v>-39.599999999999994</v>
       </c>
       <c r="Q46" s="39">
         <f>P46+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-30.2</v>
+        <v>-39.599999999999994</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -8053,23 +8142,23 @@
       </c>
       <c r="M47" s="1">
         <f>L47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-2.2500000000000036</v>
+        <v>-42.25</v>
       </c>
       <c r="N47" s="1">
         <f>M47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-2.2500000000000036</v>
+        <v>-39.700000000000003</v>
       </c>
       <c r="O47" s="1">
         <f>N47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-2.2500000000000036</v>
+        <v>-39.700000000000003</v>
       </c>
       <c r="P47" s="1">
         <f>O47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-2.2500000000000036</v>
+        <v>-39.700000000000003</v>
       </c>
       <c r="Q47" s="39">
         <f>P47+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>-2.2500000000000036</v>
+        <v>-39.700000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -8121,23 +8210,23 @@
       </c>
       <c r="M48" s="1">
         <f>L48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>14.399999999999999</v>
+        <v>23.45</v>
       </c>
       <c r="N48" s="1">
         <f>M48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>14.399999999999999</v>
+        <v>66.349999999999994</v>
       </c>
       <c r="O48" s="1">
         <f>N48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>14.399999999999999</v>
+        <v>66.349999999999994</v>
       </c>
       <c r="P48" s="1">
         <f>O48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>14.399999999999999</v>
+        <v>66.349999999999994</v>
       </c>
       <c r="Q48" s="39">
         <f>P48+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>14.399999999999999</v>
+        <v>66.349999999999994</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -8257,23 +8346,23 @@
       </c>
       <c r="M50" s="1">
         <f>L50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_11[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.7</v>
+        <v>23.5</v>
       </c>
       <c r="N50" s="1">
         <f>M50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_12[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.7</v>
+        <v>21.9</v>
       </c>
       <c r="O50" s="1">
         <f>N50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_13[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.7</v>
+        <v>21.9</v>
       </c>
       <c r="P50" s="1">
         <f>O50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_14[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.7</v>
+        <v>21.9</v>
       </c>
       <c r="Q50" s="39">
         <f>P50+VLOOKUP(MovingSum[[#This Row],[SPIELER]],Day_15[[SPIELER]:[WIN / LOSS]],2,FALSE)</f>
-        <v>13.7</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>